<commit_message>
update hello-world local search stats
</commit_message>
<xml_diff>
--- a/examples/src/main/resources/ai/timefold/solver/examples/cloudbalancing/cloudBalancing..xlsx
+++ b/examples/src/main/resources/ai/timefold/solver/examples/cloudbalancing/cloudBalancing..xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeong\workspaces\zionex\timefold-quickstarts\examples\src\main\resources\ai\timefold\solver\examples\cloudbalancing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CF5B22-5ACB-421D-9813-7AEB1097E1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3579D90E-9BF6-4174-A2A5-830BA157048D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="31785" xr2:uid="{F3B50315-B6F7-49C9-8098-BD1559159854}"/>
+    <workbookView xWindow="38295" yWindow="0" windowWidth="19410" windowHeight="31785" xr2:uid="{F3B50315-B6F7-49C9-8098-BD1559159854}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -392,46 +392,46 @@
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked4.xml</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked1.xml</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked3.xml</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked-partition4.xml</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked2.xml</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked-partition3.xml</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked-partition1.xml</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked-partition2.xml</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked-partition2.xml</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.10min.xml</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>cloudBalancingSolverConfig.fixed-random.05min.xml</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>cloudBalancingSolverConfig.xml</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="12">
                   <c:v>cloudBalancingSolverConfig.fixed-random.02min.xml</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="13">
                   <c:v>cloudBalancingSolverConfig.fixed-random.02min.xml</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.05min.xml</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.10min.xml</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked1.xml</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked2.xml</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked3.xml</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked4.xml</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked-partition1.xml</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked-partition2.xml</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked-partition2.xml</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked-partition3.xml</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>cloudBalancingSolverConfig.fixed-random.tweaked-partition4.xml</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -443,46 +443,46 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>-1730180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1738610</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1755380</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1767600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1772420</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1783670</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1794910</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1795010</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1814180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1852360</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1857160</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>-1868110</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="12">
+                  <c:v>-1871440</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>-1871540</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-1871440</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-1857160</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-1852360</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-1738610</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1772420</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1755380</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1730180</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1794910</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1814180</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-1795010</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-1783670</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-1767600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,7 +1550,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,125 +1597,129 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>-1868110</v>
+        <v>-1730180</v>
       </c>
       <c r="F3" s="7">
         <f>(MAX($E$3:$E$160)-E3)/MAX($E$3:$E$16)</f>
-        <v>-7.9720029129917117E-2</v>
+        <v>0</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
       </c>
       <c r="E4" s="6">
-        <v>-1871540</v>
+        <v>-1738610</v>
       </c>
       <c r="F4" s="7">
         <f>(MAX($E$3:$E$160)-E4)/MAX($E$3:$E$16)</f>
-        <v>-8.1702481822700526E-2</v>
+        <v>-4.8723254227883801E-3</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
       </c>
       <c r="E5" s="6">
-        <v>-1871440</v>
+        <v>-1755380</v>
       </c>
       <c r="F5" s="7">
         <f>(MAX($E$3:$E$160)-E5)/MAX($E$3:$E$16)</f>
-        <v>-8.1644684368100434E-2</v>
+        <v>-1.4564958559225051E-2</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6">
         <v>0</v>
       </c>
       <c r="E6" s="6">
-        <v>-1857160</v>
+        <v>-1767600</v>
       </c>
       <c r="F6" s="7">
         <f>(MAX($E$3:$E$160)-E6)/MAX($E$3:$E$16)</f>
-        <v>-7.339120785120623E-2</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>-2.1627807511357199E-2</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="6">
         <v>0</v>
       </c>
       <c r="E7" s="6">
-        <v>-1852360</v>
+        <v>-1772420</v>
       </c>
       <c r="F7" s="7">
         <f>(MAX($E$3:$E$160)-E7)/MAX($E$3:$E$16)</f>
-        <v>-7.0616930030401467E-2</v>
+        <v>-2.4413644823081993E-2</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>17</v>
@@ -1724,21 +1728,23 @@
         <v>0</v>
       </c>
       <c r="E8" s="6">
-        <v>-1738610</v>
+        <v>-1783670</v>
       </c>
       <c r="F8" s="7">
         <f>(MAX($E$3:$E$160)-E8)/MAX($E$3:$E$16)</f>
-        <v>-4.8723254227883801E-3</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>-3.0915858465593176E-2</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>17</v>
@@ -1747,94 +1753,96 @@
         <v>0</v>
       </c>
       <c r="E9" s="6">
-        <v>-1772420</v>
+        <v>-1794910</v>
       </c>
       <c r="F9" s="7">
         <f>(MAX($E$3:$E$160)-E9)/MAX($E$3:$E$16)</f>
-        <v>-2.4413644823081993E-2</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>-3.7412292362644352E-2</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="6">
         <v>0</v>
       </c>
       <c r="E10" s="6">
-        <v>-1755380</v>
+        <v>-1795010</v>
       </c>
       <c r="F10" s="7">
         <f>(MAX($E$3:$E$160)-E10)/MAX($E$3:$E$16)</f>
-        <v>-1.4564958559225051E-2</v>
-      </c>
-      <c r="G10" s="4"/>
+        <v>-3.7470089817244451E-2</v>
+      </c>
+      <c r="G10" s="8">
+        <v>8</v>
+      </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="6">
         <v>0</v>
       </c>
       <c r="E11" s="6">
-        <v>-1730180</v>
+        <v>-1814180</v>
       </c>
       <c r="F11" s="7">
         <f>(MAX($E$3:$E$160)-E11)/MAX($E$3:$E$16)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>-4.8549861864083506E-2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>4</v>
+      </c>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="6">
         <v>0</v>
       </c>
       <c r="E12" s="6">
-        <v>-1794910</v>
+        <v>-1852360</v>
       </c>
       <c r="F12" s="7">
         <f>(MAX($E$3:$E$160)-E12)/MAX($E$3:$E$16)</f>
-        <v>-3.7412292362644352E-2</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>14</v>
-      </c>
+        <v>-7.0616930030401467E-2</v>
+      </c>
+      <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>17</v>
@@ -1843,95 +1851,87 @@
         <v>0</v>
       </c>
       <c r="E13" s="6">
-        <v>-1814180</v>
+        <v>-1857160</v>
       </c>
       <c r="F13" s="7">
         <f>(MAX($E$3:$E$160)-E13)/MAX($E$3:$E$16)</f>
-        <v>-4.8549861864083506E-2</v>
-      </c>
-      <c r="G13" s="8">
-        <v>4</v>
-      </c>
+        <v>-7.339120785120623E-2</v>
+      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="6">
         <v>0</v>
       </c>
       <c r="E14" s="6">
-        <v>-1795010</v>
+        <v>-1868110</v>
       </c>
       <c r="F14" s="7">
         <f>(MAX($E$3:$E$160)-E14)/MAX($E$3:$E$16)</f>
-        <v>-3.7470089817244451E-2</v>
-      </c>
-      <c r="G14" s="8">
-        <v>8</v>
-      </c>
+        <v>-7.9720029129917117E-2</v>
+      </c>
+      <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="6">
         <v>0</v>
       </c>
       <c r="E15" s="6">
-        <v>-1783670</v>
+        <v>-1871440</v>
       </c>
       <c r="F15" s="7">
         <f>(MAX($E$3:$E$160)-E15)/MAX($E$3:$E$16)</f>
-        <v>-3.0915858465593176E-2</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>14</v>
-      </c>
+        <v>-8.1644684368100434E-2</v>
+      </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D16" s="6">
         <v>0</v>
       </c>
       <c r="E16" s="6">
-        <v>-1767600</v>
+        <v>-1871540</v>
       </c>
       <c r="F16" s="7">
         <f>(MAX($E$3:$E$160)-E16)/MAX($E$3:$E$16)</f>
-        <v>-2.1627807511357199E-2</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>14</v>
-      </c>
+        <v>-8.1702481822700526E-2</v>
+      </c>
+      <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H16">
-    <sortCondition ref="A3:A16"/>
+    <sortCondition descending="1" ref="E3:E16"/>
   </sortState>
   <conditionalFormatting sqref="E3:E16">
     <cfRule type="colorScale" priority="3">

</xml_diff>